<commit_message>
Major improvements to network_bayes.ado - added model AB2. Not fully tested. Also improved network_bayes_cscript.do. Still need to check all priors.
</commit_message>
<xml_diff>
--- a/package/network_bayes_parameters.xlsx
+++ b/package/network_bayes_parameters.xlsx
@@ -10,12 +10,15 @@
     <sheet name="priorparms" sheetId="1" r:id="rId1"/>
     <sheet name="parms" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">parms!$A$1:$O$33</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="115">
   <si>
     <t>Model</t>
   </si>
@@ -146,9 +149,6 @@
     <t>parameter</t>
   </si>
   <si>
-    <t>inverse wishart (f*df*I,df)</t>
-  </si>
-  <si>
     <t>I=identity</t>
   </si>
   <si>
@@ -185,9 +185,6 @@
     <t>[NT,NT]</t>
   </si>
   <si>
-    <t>Derived parameters (can be output)</t>
-  </si>
-  <si>
     <t>main effect of study</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>heterogeneity correlation in arm-based model</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Random effects</t>
   </si>
   <si>
@@ -251,20 +245,9 @@
     <t>Inverse variance matrix of contrast heterogeneity</t>
   </si>
   <si>
-    <t>Wishart (f*df*P,df)</t>
-  </si>
-  <si>
     <t>invSigmaA</t>
   </si>
   <si>
-    <t>f chosen to respect logsigCmean
-df=NT-1</t>
-  </si>
-  <si>
-    <t>f chosen to respect logsigAmean
-df=NT</t>
-  </si>
-  <si>
     <t>Inverse variance matrix of arm-specific treatment effects</t>
   </si>
   <si>
@@ -277,10 +260,6 @@
     <t>mean of effects of study, in random study effect models</t>
   </si>
   <si>
-    <t>f chosen to respect logsigCmean
-df=NT</t>
-  </si>
-  <si>
     <t>sigC2</t>
   </si>
   <si>
@@ -290,31 +269,100 @@
     <t>contrasts with reference</t>
   </si>
   <si>
-    <t>contrast heterogeneity variance</t>
-  </si>
-  <si>
-    <t>shading = default output parameter</t>
-  </si>
-  <si>
-    <t>* = model parameter without prior</t>
-  </si>
-  <si>
-    <t>x = model parameter with prior</t>
-  </si>
-  <si>
-    <t>NS = #studies</t>
-  </si>
-  <si>
-    <t>NT = #treatments</t>
-  </si>
-  <si>
-    <t>P = matrix with ones on diagonal, halves off diagonal</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
-    <t>d = derived parameter</t>
+    <t xml:space="preserve">NT </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #treatments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> derived parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> default output parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> matrix with ones on diagonal, halves off diagonal</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i </t>
+  </si>
+  <si>
+    <t>intermediate model parameter - prior must not be specified</t>
+  </si>
+  <si>
+    <t>basic model parameter - prior must be specified</t>
+  </si>
+  <si>
+    <t>sigA2</t>
+  </si>
+  <si>
+    <t>SigmaC</t>
+  </si>
+  <si>
+    <t>[NT]</t>
+  </si>
+  <si>
+    <t>arm heterogeneity variance/covariance matrix</t>
+  </si>
+  <si>
+    <t>common arm heterogeneity variance</t>
+  </si>
+  <si>
+    <t>vector of arm heterogeneity variances</t>
+  </si>
+  <si>
+    <t>common contrast heterogeneity</t>
+  </si>
+  <si>
+    <t>array of contrast heterogeneity variances</t>
+  </si>
+  <si>
+    <t>contrast heterogeneity variance/covariance matrix relative to reference</t>
+  </si>
+  <si>
+    <t>Derived parameters in Winbugs run - can be specified in parms()</t>
+  </si>
+  <si>
+    <t>Parameters derived after Winbugs run - automatically output [?]</t>
+  </si>
+  <si>
+    <t>Wishart (f*P,df)</t>
+  </si>
+  <si>
+    <t>Wishart (f*I,df)</t>
+  </si>
+  <si>
+    <t>inverse wishart (f*I,df)</t>
+  </si>
+  <si>
+    <t>f chosen to respect logsigCmean; df=NT-1</t>
+  </si>
+  <si>
+    <t>f chosen to respect logsigCmean; df=NT</t>
+  </si>
+  <si>
+    <t>f chosen to respect logsigAmean; df=NT</t>
   </si>
 </sst>
 </file>
@@ -393,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -479,6 +527,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -487,15 +547,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,20 +869,20 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1044,13 +1095,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,12 +1109,12 @@
     <col min="1" max="1" width="4.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" style="1" customWidth="1"/>
-    <col min="5" max="8" width="6.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="5" customWidth="1"/>
-    <col min="10" max="13" width="6.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="21.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" style="1" customWidth="1"/>
+    <col min="5" max="8" width="4.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" style="5" customWidth="1"/>
+    <col min="10" max="13" width="4.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.28515625" style="12" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -1101,7 +1152,7 @@
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
@@ -1109,19 +1160,19 @@
         <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
       <c r="N3" s="12" t="s">
         <v>33</v>
       </c>
@@ -1133,24 +1184,24 @@
       <c r="A4" s="7"/>
       <c r="D4" s="23"/>
       <c r="E4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="30"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
@@ -1206,36 +1257,38 @@
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="8"/>
+        <v>94</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="12" t="s">
@@ -1245,16 +1298,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" s="11">
         <v>1</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="21"/>
@@ -1262,10 +1315,10 @@
       <c r="H8" s="8"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -1276,16 +1329,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -1293,10 +1346,10 @@
       <c r="H9" s="16"/>
       <c r="I9" s="27"/>
       <c r="J9" s="27" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
@@ -1325,37 +1378,37 @@
       <c r="M10" s="8"/>
       <c r="O10" s="25"/>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
@@ -1386,13 +1439,13 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -1402,10 +1455,10 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="N13" s="18" t="s">
         <v>38</v>
@@ -1431,7 +1484,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>26</v>
       </c>
@@ -1439,25 +1492,25 @@
         <v>1</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>12</v>
+        <v>61</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="G15" s="21"/>
-      <c r="H15" s="32" t="s">
-        <v>12</v>
+      <c r="H15" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="8" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="K15" s="8"/>
       <c r="L15" s="8" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="12" t="s">
@@ -1467,7 +1520,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="11" t="s">
         <v>27</v>
@@ -1476,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="21"/>
@@ -1486,7 +1539,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="M16" s="8"/>
       <c r="N16" s="12" t="s">
@@ -1496,70 +1549,70 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="21"/>
       <c r="G17" s="21" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="12" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="9" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="12" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="D19" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="21"/>
@@ -1570,13 +1623,13 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="O19" s="22" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1594,13 +1647,13 @@
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
       <c r="N20" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O20" s="18"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1620,16 +1673,16 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
@@ -1646,59 +1699,63 @@
       <c r="A23" s="20"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="H23" s="21"/>
       <c r="I23" s="9"/>
       <c r="J23" s="21" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="7"/>
       <c r="O23" s="22"/>
     </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
+      <c r="L24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>94</v>
+      </c>
       <c r="N24" s="14"/>
       <c r="O24" s="18"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -1718,134 +1775,340 @@
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="11" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="H26" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="I26" s="32" t="s">
-        <v>97</v>
+        <v>101</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
+      <c r="M26" s="21" t="s">
+        <v>83</v>
+      </c>
       <c r="N26" s="7"/>
       <c r="O26" s="22"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="22"/>
+        <v>98</v>
+      </c>
+      <c r="C27" s="11">
+        <v>1</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>102</v>
+      </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
-      <c r="I27" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="M27" s="29"/>
       <c r="N27" s="7"/>
       <c r="O27" s="22"/>
     </row>
-    <row r="28" spans="1:15" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="H28" s="16"/>
-      <c r="I28" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="18"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N28" s="7"/>
+      <c r="O28" s="22"/>
+    </row>
+    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
       <c r="N29" s="7"/>
       <c r="O29" s="22"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="11">
+        <v>1</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="K30" s="29"/>
+      <c r="L30" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="M30" s="29"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="22"/>
+    </row>
+    <row r="31" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="C31" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="16"/>
+      <c r="I31" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="J31" s="16"/>
+      <c r="K31" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L31" s="16"/>
+      <c r="M31" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="N31" s="14"/>
+      <c r="O31" s="18"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="22"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="M33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="N33" s="14"/>
+      <c r="O33" s="18"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="22"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="22"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="22"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="22"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="32"/>
+      <c r="B43" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1857,7 +2120,7 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="67" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;F &amp;A&amp;R&amp;D &amp;T</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Small changes made 23jun2018
</commit_message>
<xml_diff>
--- a/package/network_bayes_parameters.xlsx
+++ b/package/network_bayes_parameters.xlsx
@@ -10,15 +10,12 @@
     <sheet name="priorparms" sheetId="1" r:id="rId1"/>
     <sheet name="parms" sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">parms!$A$1:$O$33</definedName>
-  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="113">
   <si>
     <t>Model</t>
   </si>
@@ -149,9 +146,6 @@
     <t>parameter</t>
   </si>
   <si>
-    <t>I=identity</t>
-  </si>
-  <si>
     <t>AB4</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>NS</t>
   </si>
   <si>
-    <t>NT-1</t>
-  </si>
-  <si>
     <t>NT</t>
   </si>
   <si>
@@ -194,9 +185,6 @@
     <t>muC</t>
   </si>
   <si>
-    <t>overall treatment effect relative to treatment 1</t>
-  </si>
-  <si>
     <t>muA</t>
   </si>
   <si>
@@ -263,12 +251,6 @@
     <t>sigC2</t>
   </si>
   <si>
-    <t>diff</t>
-  </si>
-  <si>
-    <t>contrasts with reference</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -323,30 +305,15 @@
     <t>[NT]</t>
   </si>
   <si>
-    <t>arm heterogeneity variance/covariance matrix</t>
+    <t>arm heterogeneity variance matrix</t>
   </si>
   <si>
     <t>common arm heterogeneity variance</t>
   </si>
   <si>
-    <t>vector of arm heterogeneity variances</t>
-  </si>
-  <si>
     <t>common contrast heterogeneity</t>
   </si>
   <si>
-    <t>array of contrast heterogeneity variances</t>
-  </si>
-  <si>
-    <t>contrast heterogeneity variance/covariance matrix relative to reference</t>
-  </si>
-  <si>
-    <t>Derived parameters in Winbugs run - can be specified in parms()</t>
-  </si>
-  <si>
-    <t>Parameters derived after Winbugs run - automatically output [?]</t>
-  </si>
-  <si>
     <t>Wishart (f*P,df)</t>
   </si>
   <si>
@@ -363,6 +330,30 @@
   </si>
   <si>
     <t>f chosen to respect logsigAmean; df=NT</t>
+  </si>
+  <si>
+    <t>overall treatment effect relative to reference treatment</t>
+  </si>
+  <si>
+    <t>array of contrast heterogeneity variances (zeroes on diagonal)</t>
+  </si>
+  <si>
+    <t>contrast heterogeneity variance matrix relative to reference</t>
+  </si>
+  <si>
+    <t>array of arm heterogeneity variances</t>
+  </si>
+  <si>
+    <t>For basic parameters</t>
+  </si>
+  <si>
+    <t>Contrast heterogeneity variance</t>
+  </si>
+  <si>
+    <t>Arm heterogeneity variance</t>
+  </si>
+  <si>
+    <t>identity matrix</t>
   </si>
 </sst>
 </file>
@@ -441,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -547,6 +538,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,13 +1089,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1103,7 @@
     <col min="1" max="1" width="4.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="1" customWidth="1"/>
     <col min="5" max="8" width="4.7109375" style="4" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" style="5" customWidth="1"/>
     <col min="10" max="13" width="4.7109375" style="4" customWidth="1"/>
@@ -1160,7 +1154,7 @@
         <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>0</v>
@@ -1173,35 +1167,39 @@
       <c r="K3" s="35"/>
       <c r="L3" s="35"/>
       <c r="M3" s="35"/>
-      <c r="N3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="N3" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="O3" s="36"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="D4" s="23"/>
       <c r="E4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>45</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>46</v>
       </c>
       <c r="G4" s="34"/>
       <c r="H4" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" s="34"/>
       <c r="J4" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M4" s="34"/>
+      <c r="N4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
@@ -1260,34 +1258,34 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -1301,13 +1299,13 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" s="11">
         <v>1</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="21"/>
@@ -1315,10 +1313,10 @@
       <c r="H8" s="8"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -1329,16 +1327,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -1346,15 +1344,15 @@
       <c r="H9" s="16"/>
       <c r="I9" s="27"/>
       <c r="J9" s="27" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O9" s="28" t="s">
         <v>21</v>
@@ -1378,40 +1376,44 @@
       <c r="M10" s="8"/>
       <c r="O10" s="25"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
+        <v>105</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>78</v>
+      </c>
       <c r="N11" s="18" t="s">
         <v>37</v>
       </c>
@@ -1439,13 +1441,13 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -1455,10 +1457,10 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N13" s="18" t="s">
         <v>38</v>
@@ -1469,650 +1471,530 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="22"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="8"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="22"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
       <c r="B15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="11">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>93</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="21"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="30" t="s">
-        <v>93</v>
-      </c>
+      <c r="H15" s="21"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="O15" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="22"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="11">
-        <v>1</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="8"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="21"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="21"/>
+      <c r="J16" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="22"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17" s="14"/>
+      <c r="O17" s="18"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="D19" s="1" t="s">
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="K19" s="8"/>
+      <c r="L19" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="N19" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="N19" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="O19" s="22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="O20" s="18"/>
+      <c r="C20" s="11">
+        <v>1</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="M20" s="29"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="22"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="8"/>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="22"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
       <c r="B22" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="C22" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="22"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="11"/>
       <c r="C23" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" s="21"/>
+        <v>51</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="K23" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
       <c r="N23" s="7"/>
       <c r="O23" s="22"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="17" t="s">
-        <v>67</v>
+    <row r="24" spans="1:15" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24" s="27" t="s">
-        <v>94</v>
+      <c r="G24" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>94</v>
+      <c r="K24" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="L24" s="16"/>
+      <c r="M24" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="N24" s="14"/>
       <c r="O24" s="18"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="22"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="22"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+    </row>
+    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
       <c r="B26" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
-      <c r="M26" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="N26" s="7"/>
-      <c r="O26" s="22"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="11">
-        <v>1</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="O26" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="D27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="M27" s="29"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="22"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="O27" s="22" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="C28" s="11" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29" t="s">
-        <v>83</v>
+      <c r="I28" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21" t="s">
+        <v>78</v>
       </c>
       <c r="N28" s="7"/>
       <c r="O28" s="22"/>
     </row>
-    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>53</v>
+        <v>93</v>
+      </c>
+      <c r="C29" s="11">
+        <v>1</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
+      <c r="J29" s="30" t="s">
+        <v>78</v>
+      </c>
       <c r="K29" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="L29" s="29"/>
+        <v>78</v>
+      </c>
+      <c r="L29" s="29" t="s">
+        <v>78</v>
+      </c>
       <c r="M29" s="29"/>
       <c r="N29" s="7"/>
       <c r="O29" s="22"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="11" t="s">
+      <c r="A30" s="26"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N30" s="14"/>
+      <c r="O30" s="18"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="22"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="11">
-        <v>1</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="K30" s="29"/>
-      <c r="L30" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="M30" s="29"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="22"/>
-    </row>
-    <row r="31" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="C31" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" s="16"/>
-      <c r="I31" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="L31" s="16"/>
-      <c r="M31" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="N31" s="14"/>
-      <c r="O31" s="18"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="22"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="17" t="s">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="18" t="s">
+      <c r="I35" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="J33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="K33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="L33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="M33" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="N33" s="14"/>
-      <c r="O33" s="18"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="22"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="22"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="22"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="22"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>92</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="N3:O3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
@@ -2120,7 +2002,7 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;F &amp;A&amp;R&amp;D &amp;T</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Edited network bayes to make analysisforpaper.do work - involved coordinating parameters in model, set & post-processed. Now nicely matches the spreadsheet. Next going to check the full analysis works.
</commit_message>
<xml_diff>
--- a/package/network_bayes_parameters.xlsx
+++ b/package/network_bayes_parameters.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="123">
   <si>
     <t>Model</t>
   </si>
@@ -146,21 +146,6 @@
     <t>parameter</t>
   </si>
   <si>
-    <t>AB4</t>
-  </si>
-  <si>
-    <t>CB1</t>
-  </si>
-  <si>
-    <t>CB2</t>
-  </si>
-  <si>
-    <t>CB3</t>
-  </si>
-  <si>
-    <t>AB2</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -191,9 +176,6 @@
     <t>mean for each treatment</t>
   </si>
   <si>
-    <t>SD of common contrast heterogeneity</t>
-  </si>
-  <si>
     <t>heterogeneity correlation in arm-based model</t>
   </si>
   <si>
@@ -236,15 +218,6 @@
     <t>invSigmaA</t>
   </si>
   <si>
-    <t>Inverse variance matrix of arm-specific treatment effects</t>
-  </si>
-  <si>
-    <t>Inverse variance matrix of arm-specific treatment means</t>
-  </si>
-  <si>
-    <t>SD of effects of study, in random study effect models</t>
-  </si>
-  <si>
     <t>mean of effects of study, in random study effect models</t>
   </si>
   <si>
@@ -311,9 +284,6 @@
     <t>common arm heterogeneity variance</t>
   </si>
   <si>
-    <t>common contrast heterogeneity</t>
-  </si>
-  <si>
     <t>Wishart (f*P,df)</t>
   </si>
   <si>
@@ -326,34 +296,94 @@
     <t>f chosen to respect logsigCmean; df=NT-1</t>
   </si>
   <si>
-    <t>f chosen to respect logsigCmean; df=NT</t>
-  </si>
-  <si>
-    <t>f chosen to respect logsigAmean; df=NT</t>
-  </si>
-  <si>
     <t>overall treatment effect relative to reference treatment</t>
   </si>
   <si>
-    <t>array of contrast heterogeneity variances (zeroes on diagonal)</t>
-  </si>
-  <si>
     <t>contrast heterogeneity variance matrix relative to reference</t>
   </si>
   <si>
-    <t>array of arm heterogeneity variances</t>
-  </si>
-  <si>
     <t>For basic parameters</t>
   </si>
   <si>
-    <t>Contrast heterogeneity variance</t>
-  </si>
-  <si>
-    <t>Arm heterogeneity variance</t>
-  </si>
-  <si>
     <t>identity matrix</t>
+  </si>
+  <si>
+    <t>b/d</t>
+  </si>
+  <si>
+    <t>d/b</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>sigA2prior</t>
+  </si>
+  <si>
+    <t>(use sigAprior)</t>
+  </si>
+  <si>
+    <t>sigC2prior</t>
+  </si>
+  <si>
+    <t>(use sigCprior)</t>
+  </si>
+  <si>
+    <t>common contrast heterogeneity variance</t>
+  </si>
+  <si>
+    <t>common contrast heterogeneity SD</t>
+  </si>
+  <si>
+    <t>array of arm heterogeneity SDs</t>
+  </si>
+  <si>
+    <t>SD of effects of study</t>
+  </si>
+  <si>
+    <t>inverse variance matrix of arm-specific treatment effects</t>
+  </si>
+  <si>
+    <t>inverse variance matrix of arm-specific treatment means</t>
+  </si>
+  <si>
+    <t>f chosen to respect logsigCmean or logsigC2mean; df=NT</t>
+  </si>
+  <si>
+    <t>f chosen to respect logsigAmean or logsigA2mean; df=NT</t>
+  </si>
+  <si>
+    <t>Sigma - var/cov matrix</t>
+  </si>
+  <si>
+    <t>sig2 - variance or array of variances</t>
+  </si>
+  <si>
+    <t>sig - SD or array of SDs</t>
+  </si>
+  <si>
+    <t>array of contrast heterogeneity SDs (zeroes on diagonal)</t>
+  </si>
+  <si>
+    <t>1CB</t>
+  </si>
+  <si>
+    <t>2CB</t>
+  </si>
+  <si>
+    <t>2AB</t>
+  </si>
+  <si>
+    <t>3CB</t>
+  </si>
+  <si>
+    <t>4AB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arm heterogeneity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contrast heterogeneity </t>
   </si>
 </sst>
 </file>
@@ -432,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -515,9 +545,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -530,17 +557,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -863,20 +905,20 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1092,10 +1134,10 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1150,7 @@
     <col min="9" max="9" width="4.7109375" style="5" customWidth="1"/>
     <col min="10" max="13" width="4.7109375" style="4" customWidth="1"/>
     <col min="14" max="14" width="21.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.28515625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" style="12" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -1154,46 +1196,46 @@
         <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="O3" s="36"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="O3" s="35"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="D4" s="23"/>
       <c r="E4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="34"/>
+        <v>116</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="M4" s="36"/>
       <c r="N4" s="12" t="s">
         <v>33</v>
       </c>
@@ -1258,34 +1300,34 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -1297,186 +1339,180 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="17">
+        <v>1</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="O9" s="25"/>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="L10" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="22"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="11">
-        <v>1</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="17">
-        <v>1</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="O9" s="28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="O10" s="25"/>
-    </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="J11" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="K11" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="L11" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="O11" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="N13" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="O13" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="21"/>
+      <c r="D14" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
@@ -1490,174 +1526,184 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
-      <c r="B15" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+        <v>57</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="H15" s="21"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
+      <c r="J15" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="7"/>
       <c r="O15" s="22"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="22"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="N16" s="14"/>
+      <c r="O16" s="18"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="I17" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="N17" s="14"/>
-      <c r="O17" s="18"/>
+      <c r="A17" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="21"/>
+      <c r="B18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="G18" s="21"/>
-      <c r="H18" s="8"/>
+      <c r="H18" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="I18" s="9"/>
-      <c r="J18" s="8"/>
+      <c r="J18" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
+      <c r="L18" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="M18" s="8"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="11">
-        <v>1</v>
+      <c r="N18" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="K19" s="8"/>
-      <c r="L19" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="M19" s="8"/>
-      <c r="N19" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="O19" s="25" t="s">
-        <v>21</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="32"/>
+      <c r="I19" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="32"/>
+      <c r="K19" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="32"/>
+      <c r="M19" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="N19" s="7"/>
+      <c r="O19" s="22"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="11" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C20" s="11">
         <v>1</v>
       </c>
       <c r="D20" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="F20" s="9" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="M20" s="29"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="22"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="M20" s="28"/>
+      <c r="N20" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="11" t="s">
         <v>27</v>
@@ -1666,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="21"/>
@@ -1676,7 +1722,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="M21" s="8"/>
       <c r="N21" s="12" t="s">
@@ -1689,234 +1735,242 @@
     <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="21"/>
       <c r="G22" s="21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="9"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="18"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L25" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="M25" s="32"/>
+      <c r="N25" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="O22" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="22"/>
-    </row>
-    <row r="24" spans="1:15" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="18" t="s">
+      <c r="C26" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" s="16"/>
-      <c r="I24" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="N24" s="14"/>
-      <c r="O24" s="18"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-    </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="9" t="s">
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="N26" s="7"/>
+      <c r="O26" s="22"/>
+    </row>
+    <row r="27" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="11">
+        <v>1</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="12" t="s">
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L27" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="M27" s="32"/>
+      <c r="N27" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="O26" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="D27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="N27" s="22" t="s">
+      <c r="O27" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="O27" s="22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+    </row>
+    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
       <c r="B28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+        <v>66</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
       <c r="I28" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
-      <c r="M28" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="N28" s="7"/>
-      <c r="O28" s="22"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="11">
-        <v>1</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="D29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="K29" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="L29" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="M29" s="29"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="22"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N29" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="O29" s="22" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
-      <c r="B30" s="17"/>
+      <c r="B30" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="C30" s="17" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
       <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
+      <c r="I30" s="27" t="s">
+        <v>69</v>
+      </c>
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
       <c r="L30" s="16"/>
-      <c r="M30" s="16" t="s">
-        <v>78</v>
+      <c r="M30" s="27" t="s">
+        <v>69</v>
       </c>
       <c r="N30" s="14"/>
       <c r="O30" s="18"/>
@@ -1926,71 +1980,88 @@
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="22"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
       <c r="N31" s="7"/>
       <c r="O31" s="22"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="O32" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="O33" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="O34" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>